<commit_message>
Iin this commit created new class to fetch the data from the excell using IEnumerable
</commit_message>
<xml_diff>
--- a/SAIPCsharp/file/dataex.xlsx
+++ b/SAIPCsharp/file/dataex.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>one</t>
   </si>
@@ -34,6 +34,24 @@
   </si>
   <si>
     <t>six</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+  <si>
+    <t>s6</t>
   </si>
 </sst>
 </file>
@@ -372,42 +390,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>